<commit_message>
added more spaces here and there
</commit_message>
<xml_diff>
--- a/Linear Single Step/output.xlsx
+++ b/Linear Single Step/output.xlsx
@@ -214,22 +214,22 @@
     <t>MethaneHubUsage</t>
   </si>
   <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>keroseneUsage</t>
+  </si>
+  <si>
     <t>tkm-N2Usage</t>
   </si>
   <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
     <t>tkm-N3Usage</t>
-  </si>
-  <si>
-    <t>tkm-SZMUsage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>keroseneUsage</t>
   </si>
 </sst>
 </file>
@@ -816,49 +816,49 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2969344.144413812</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1177.369968223092</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>174.6711445919873</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>2041.829144604735</v>
+        <v>539.1010105329111</v>
       </c>
       <c r="G2">
-        <v>207.0328368011472</v>
+        <v>50.01256931675417</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>865.6153846153844</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>502.6153846153845</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>229.338685832091</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>74.58168644946049</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>154.7569993826305</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>171.0515151515152</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>171.0515151515152</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -897,25 +897,25 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>1491.73788300216</v>
+        <v>360.0785051643636</v>
       </c>
       <c r="AD2">
-        <v>460.9884430110843</v>
+        <v>111.2742602764874</v>
       </c>
       <c r="AE2">
-        <v>1030.749439991076</v>
+        <v>248.8042448878763</v>
       </c>
       <c r="AF2">
-        <v>166.8965517241379</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>40.88965517241379</v>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>5.006896551724139</v>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
         <v>0</v>
@@ -924,10 +924,10 @@
         <v>0</v>
       </c>
       <c r="AL2">
-        <v>0</v>
+        <v>49.99999999999999</v>
       </c>
       <c r="AM2">
-        <v>0</v>
+        <v>49.99999999999999</v>
       </c>
       <c r="AN2">
         <v>50</v>
@@ -936,22 +936,22 @@
         <v>50</v>
       </c>
       <c r="AP2">
-        <v>396.2195511974985</v>
+        <v>377.254694783643</v>
       </c>
       <c r="AQ2">
-        <v>396.2195511974985</v>
+        <v>377.254694783643</v>
       </c>
       <c r="AR2">
-        <v>442.5804488025015</v>
+        <v>377.665305216357</v>
       </c>
       <c r="AS2">
-        <v>442.5804488025015</v>
+        <v>377.665305216357</v>
       </c>
       <c r="AT2">
-        <v>8</v>
+        <v>7.2</v>
       </c>
       <c r="AU2">
-        <v>8</v>
+        <v>7.2</v>
       </c>
       <c r="AV2">
         <v>26.2</v>
@@ -960,28 +960,28 @@
         <v>26.2</v>
       </c>
       <c r="AX2">
-        <v>123.8</v>
+        <v>111.42</v>
       </c>
       <c r="AY2">
-        <v>123.8</v>
+        <v>111.42</v>
       </c>
       <c r="AZ2">
-        <v>388.5</v>
+        <v>349.65</v>
       </c>
       <c r="BA2">
-        <v>388.5</v>
+        <v>349.65</v>
       </c>
       <c r="BB2">
-        <v>0</v>
+        <v>83.88</v>
       </c>
       <c r="BC2">
-        <v>0</v>
+        <v>83.88</v>
       </c>
       <c r="BD2">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="BE2">
-        <v>0</v>
+        <v>0.7999999999999998</v>
       </c>
       <c r="BF2">
         <v>0</v>
@@ -990,46 +990,46 @@
         <v>0</v>
       </c>
       <c r="BH2">
-        <v>0</v>
+        <v>12.38</v>
       </c>
       <c r="BI2">
-        <v>0</v>
+        <v>12.38</v>
       </c>
       <c r="BJ2">
-        <v>0</v>
+        <v>38.85</v>
       </c>
       <c r="BK2">
-        <v>0</v>
+        <v>38.85000000000002</v>
       </c>
       <c r="BL2">
-        <v>501.8780981834981</v>
+        <v>477.8559467259478</v>
       </c>
       <c r="BM2">
-        <v>1085.7563365428</v>
+        <v>956.1766288858913</v>
       </c>
       <c r="BN2">
         <v>121</v>
       </c>
       <c r="BO2">
-        <v>0</v>
+        <v>171.0515151515152</v>
       </c>
       <c r="BP2">
+        <v>838.8</v>
+      </c>
+      <c r="BQ2">
+        <v>8</v>
+      </c>
+      <c r="BR2">
+        <v>121</v>
+      </c>
+      <c r="BS2">
         <v>26.2</v>
       </c>
-      <c r="BQ2">
+      <c r="BT2">
+        <v>388.5</v>
+      </c>
+      <c r="BU2">
         <v>123.8</v>
-      </c>
-      <c r="BR2">
-        <v>388.5</v>
-      </c>
-      <c r="BS2">
-        <v>838.8</v>
-      </c>
-      <c r="BT2">
-        <v>8</v>
-      </c>
-      <c r="BU2">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified lss output, apparently
Just ignore this
</commit_message>
<xml_diff>
--- a/Linear Single Step/output.xlsx
+++ b/Linear Single Step/output.xlsx
@@ -214,22 +214,22 @@
     <t>MethaneHubUsage</t>
   </si>
   <si>
+    <t>tkm-N3Usage</t>
+  </si>
+  <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
     <t>tkm-N2Usage</t>
   </si>
   <si>
-    <t>tkm-N3Usage</t>
+    <t>keroseneUsage</t>
   </si>
   <si>
     <t>tkm-SZMUsage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>keroseneUsage</t>
   </si>
 </sst>
 </file>
@@ -1014,22 +1014,22 @@
         <v>0</v>
       </c>
       <c r="BP2">
+        <v>123.8</v>
+      </c>
+      <c r="BQ2">
+        <v>8</v>
+      </c>
+      <c r="BR2">
+        <v>838.8</v>
+      </c>
+      <c r="BS2">
         <v>26.2</v>
       </c>
-      <c r="BQ2">
-        <v>123.8</v>
-      </c>
-      <c r="BR2">
+      <c r="BT2">
+        <v>121</v>
+      </c>
+      <c r="BU2">
         <v>388.5</v>
-      </c>
-      <c r="BS2">
-        <v>838.8</v>
-      </c>
-      <c r="BT2">
-        <v>8</v>
-      </c>
-      <c r="BU2">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>